<commit_message>
import products image fix
</commit_message>
<xml_diff>
--- a/public/backend/assets/import-samples/sample_product.xlsx
+++ b/public/backend/assets/import-samples/sample_product.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohanes/Desktop/Playground/Projects/ratna/public/backend/assets/import-samples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="4740" yWindow="1580" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
@@ -11,6 +16,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -97,6 +105,18 @@
   </si>
   <si>
     <t>parent_sku</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>2017-05-15 10:00:00</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Product description (Can be in HTML)</t>
   </si>
 </sst>
 </file>
@@ -162,6 +182,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -487,155 +512,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
         <v>2250000</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>1000</v>
       </c>
-      <c r="J2" s="2" t="b">
+      <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="3" t="b">
+      <c r="M2" s="3">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="b">
+      <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>2</v>
       </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3">
         <v>1440000</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>1000</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="3" t="b">
+      <c r="M3" s="3">
         <v>1</v>
       </c>
-      <c r="M3" s="2" t="b">
+      <c r="N3" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>